<commit_message>
Add detailed description of the df.columns in Legend_Wind_Solar_Data.xlsx. Add some information in READ_ME file.
</commit_message>
<xml_diff>
--- a/data/Legend_Wind_Solar_Data.xlsx
+++ b/data/Legend_Wind_Solar_Data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elise/PycharmProjects/WorldEROI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49288527-0AAB-2240-A981-289CE32F3751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3269DDC9-68F7-754B-9A75-1BC27B820502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{2C324711-0E01-5A4C-8179-CAD4FD71C5ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{2C324711-0E01-5A4C-8179-CAD4FD71C5ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cell" sheetId="1" r:id="rId1"/>
-    <sheet name="Land Cover Classes" sheetId="2" r:id="rId2"/>
-    <sheet name="Slope Gradients" sheetId="3" r:id="rId3"/>
+    <sheet name="df.columns" sheetId="4" r:id="rId1"/>
+    <sheet name="Cell" sheetId="1" r:id="rId2"/>
+    <sheet name="Land Cover Classes" sheetId="2" r:id="rId3"/>
+    <sheet name="Slope Gradients" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="289">
   <si>
     <t>True</t>
   </si>
@@ -262,9 +263,6 @@
     <t>LC1 (/5625)</t>
   </si>
   <si>
-    <t>Column Index</t>
-  </si>
-  <si>
     <t>EROI_min_1_vr</t>
   </si>
   <si>
@@ -524,13 +522,394 @@
   </si>
   <si>
     <t>CSP (Max slope = 2%)</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>GHI</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>protected</t>
+  </si>
+  <si>
+    <t>Elev</t>
+  </si>
+  <si>
+    <t>DistCoast</t>
+  </si>
+  <si>
+    <t>WindMean71</t>
+  </si>
+  <si>
+    <t>WindStd71</t>
+  </si>
+  <si>
+    <t>WindMean125</t>
+  </si>
+  <si>
+    <t>WindStd125</t>
+  </si>
+  <si>
+    <t>Dissip</t>
+  </si>
+  <si>
+    <t>v_r_opti</t>
+  </si>
+  <si>
+    <t>n_opti</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>wind_sf_onshore</t>
+  </si>
+  <si>
+    <t>pv_sf</t>
+  </si>
+  <si>
+    <t>csp_sf</t>
+  </si>
+  <si>
+    <t>wind_sf_offshore</t>
+  </si>
+  <si>
+    <t>slope_pv_sf</t>
+  </si>
+  <si>
+    <t>slope_csp_sf</t>
+  </si>
+  <si>
+    <t>wind_area_onshore</t>
+  </si>
+  <si>
+    <t>wind_area_offshore</t>
+  </si>
+  <si>
+    <t>pv_area</t>
+  </si>
+  <si>
+    <t>csp_area</t>
+  </si>
+  <si>
+    <t>WindMean100</t>
+  </si>
+  <si>
+    <t>WindStd100</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>air_density</t>
+  </si>
+  <si>
+    <t>inputs_gw_onshore</t>
+  </si>
+  <si>
+    <t>inputs_gw_offshore</t>
+  </si>
+  <si>
+    <t>wind_onshore_e</t>
+  </si>
+  <si>
+    <t>wind_offshore_e</t>
+  </si>
+  <si>
+    <t>wind_e</t>
+  </si>
+  <si>
+    <t>wind_onshore_gw</t>
+  </si>
+  <si>
+    <t>wind_offshore_gw</t>
+  </si>
+  <si>
+    <t>wind_onshore_e_in</t>
+  </si>
+  <si>
+    <t>wind_offshore_e_in</t>
+  </si>
+  <si>
+    <t>wind_e_in</t>
+  </si>
+  <si>
+    <t>wind_onshore_eroi</t>
+  </si>
+  <si>
+    <t>wind_offshore_eroi</t>
+  </si>
+  <si>
+    <t>wind_eroi</t>
+  </si>
+  <si>
+    <t>wind_cf</t>
+  </si>
+  <si>
+    <t>pv_gw</t>
+  </si>
+  <si>
+    <t>pv_e</t>
+  </si>
+  <si>
+    <t>pv_e_in</t>
+  </si>
+  <si>
+    <t>pv_eroi</t>
+  </si>
+  <si>
+    <t>pv_cf</t>
+  </si>
+  <si>
+    <t>csp_sm</t>
+  </si>
+  <si>
+    <t>csp_eff</t>
+  </si>
+  <si>
+    <t>csp_e</t>
+  </si>
+  <si>
+    <t>csp_gw</t>
+  </si>
+  <si>
+    <t>csp_e_in</t>
+  </si>
+  <si>
+    <t>Column name</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>kWh/m2/day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average direction normal irradiation from the Global Solar Atlas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average direct normal irradiation from the Global Solar Atlas </t>
+  </si>
+  <si>
+    <t>/ 10000</t>
+  </si>
+  <si>
+    <t>See 'Slope Gradients'!A1</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of protected area (from </t>
+  </si>
+  <si>
+    <t>See 'Land Cover Classes'!A1</t>
+  </si>
+  <si>
+    <t>/ 5625</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>W/m^2</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>Elevation (water depth (&lt; 0) or altitude (&gt; 0))</t>
+  </si>
+  <si>
+    <t>Distance to the nearest coast</t>
+  </si>
+  <si>
+    <t>Mean wind speed at 71 m height</t>
+  </si>
+  <si>
+    <t>Standard deviation of the wind speed at 71 m height</t>
+  </si>
+  <si>
+    <t>Mean wind speed at 125 m height</t>
+  </si>
+  <si>
+    <t>Standard deviation of the wind speed at 125 m height</t>
+  </si>
+  <si>
+    <t>Optimal rated wind speed of the wind turbine</t>
+  </si>
+  <si>
+    <t>Optimal spacing between consecutive rows of wind turbines, in number of rotor diameter</t>
+  </si>
+  <si>
+    <t># RD</t>
+  </si>
+  <si>
+    <t>Suitability factor for pv</t>
+  </si>
+  <si>
+    <t>Suitability factor for csp</t>
+  </si>
+  <si>
+    <t>Suitability factor for offshore wind</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>Mean wind speed at 100 m height, calculated as the arithmetic mean of the wind speeds at 71 and 125 m from ERA dataset.</t>
+  </si>
+  <si>
+    <t>Standard deviation of the wind speed at 100 m height</t>
+  </si>
+  <si>
+    <t>Hub height (elevation + 100 m)</t>
+  </si>
+  <si>
+    <t>Pressure at hub height (100 m)</t>
+  </si>
+  <si>
+    <t>Air density = P/RT at hub height (100 m)</t>
+  </si>
+  <si>
+    <t>Weibull parameters (k and c) of the wind speed distribution, approximated based on mean and std of wind speed at 100 m height</t>
+  </si>
+  <si>
+    <t>Additionnal suitability factor for CSP based on average slope of the terrain (should be &lt;= 2%)</t>
+  </si>
+  <si>
+    <t>Additionnal suitability factor for PV based on average slope of the terrain (should be &lt;= 30%)</t>
+  </si>
+  <si>
+    <t>Total area computed based on the latitude and longitude of the center and the resolution of the grid (= 2 PI R^2 *|sin(lat1)-sin(lat2)| * |lon1 - lon2| / 360)</t>
+  </si>
+  <si>
+    <t>Suitability factor for onshore wind (i.e. % of the total cell's area considered as suitable for wind farm installation, based on criteria defined in suitability_factors/wind_onshore)</t>
+  </si>
+  <si>
+    <t>Total area suitable for onshore wind farm installation ( = suitabiliy factor * area)</t>
+  </si>
+  <si>
+    <t>Total area suitable for csp power plants installation ( = suitabiliy factor * area)</t>
+  </si>
+  <si>
+    <t>Total area suitable for pv power plants installation ( = suitabiliy factor * area)</t>
+  </si>
+  <si>
+    <t>Total area suitable for offshore wind farm installation ( = suitabiliy factor * area)</t>
+  </si>
+  <si>
+    <t>J / GW</t>
+  </si>
+  <si>
+    <t>EJ / year</t>
+  </si>
+  <si>
+    <t>GW installed</t>
+  </si>
+  <si>
+    <t>Total energy inputs over the life time of 1 GW onshore wind farm (depending on distance for transport)</t>
+  </si>
+  <si>
+    <t>Total energy inputs over the life time of 1 GW offshore wind farm (depending on distance to coast and water depth)</t>
+  </si>
+  <si>
+    <t>Total wind onshore energy produced when the suitable area is covered with power plants (*(1-operational energy inputs) if remove_operational_e is set to True in model_params file)</t>
+  </si>
+  <si>
+    <t>Total wind offshore energy produced when the suitable area is covered with power plants (*(1-operational energy inputs) if remove_operational_e is set to True in model_params file)</t>
+  </si>
+  <si>
+    <t>Total wind energy produced when the suitable area is covered with power plants (*(1-operational energy inputs) if remove_operational_e is set to True in model_params file)</t>
+  </si>
+  <si>
+    <t>Onshore wind installed capacity corresponding to the energy produced</t>
+  </si>
+  <si>
+    <t>Offshore wind installed capacity corresponding to the energy produced</t>
+  </si>
+  <si>
+    <t>PV installed capacity corresponding to the energy produced</t>
+  </si>
+  <si>
+    <t>CSP installed capacity corresponding to the energy produced</t>
+  </si>
+  <si>
+    <t>Total CSP energy produced when the suitable area is covered with power plants (*(1-operational energy inputs) if remove_operational_e is set to True in model_params file)</t>
+  </si>
+  <si>
+    <t>Total PV energy produced when the suitable area is covered with power plants (*(1-operational energy inputs) if remove_operational_e is set to True in model_params file)</t>
+  </si>
+  <si>
+    <t>Total energy inputs for the installed capacity considered, distributed of the life time of a power plants</t>
+  </si>
+  <si>
+    <t>Gross energy outputs / (Energy inputs + operational energy if calculate_geer is set to False in model_params file)</t>
+  </si>
+  <si>
+    <t>csp_eroi</t>
+  </si>
+  <si>
+    <t>Total life time efficiency of a CSP power plants for the optimal solar multiple considered and the average DNI of the cell</t>
+  </si>
+  <si>
+    <t>Average capacity factor of a PV power plant on the cell</t>
+  </si>
+  <si>
+    <t>Average capacity factor of a wind power plant on the cell</t>
+  </si>
+  <si>
+    <t>csp_cf</t>
+  </si>
+  <si>
+    <t>Average capacity factor of a CSP power plant on the cell</t>
+  </si>
+  <si>
+    <t>Optimal solar multiple (i.e. the one that maximises the EROI for the local DNI and the CSP technology selected in model_params file)</t>
+  </si>
+  <si>
+    <t>Column Index (in file wind_solar_0_75)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -593,6 +972,22 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -611,10 +1006,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -631,8 +1027,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -944,16 +1344,950 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FD056C-5D0E-DF4C-88F1-1298AE9698DA}">
-  <dimension ref="A1:C162"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154C765A-BDEF-F140-9E2C-248EF4A6F5EB}">
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="109.5" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" hidden="1">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" hidden="1">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" hidden="1">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" hidden="1">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" hidden="1">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" hidden="1">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" hidden="1">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" hidden="1">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" hidden="1">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" hidden="1">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" hidden="1">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" hidden="1">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" hidden="1">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" hidden="1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" hidden="1">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" hidden="1">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" hidden="1">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" hidden="1">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" hidden="1">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" hidden="1">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" hidden="1">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" hidden="1">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" hidden="1">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" hidden="1">
+      <c r="A38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" hidden="1">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" hidden="1">
+      <c r="A41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" hidden="1">
+      <c r="A42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" hidden="1">
+      <c r="A43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43" t="s">
+        <v>233</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" hidden="1">
+      <c r="A44" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" hidden="1">
+      <c r="A45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" hidden="1">
+      <c r="A46" t="s">
+        <v>174</v>
+      </c>
+      <c r="B46" t="s">
+        <v>233</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" hidden="1">
+      <c r="A47" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" t="s">
+        <v>245</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" t="s">
+        <v>234</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" t="s">
+        <v>234</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>183</v>
+      </c>
+      <c r="B55" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" t="s">
+        <v>236</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" t="s">
+        <v>236</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" hidden="1">
+      <c r="A59" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" t="s">
+        <v>233</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" hidden="1">
+      <c r="A60" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60" t="s">
+        <v>234</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" hidden="1">
+      <c r="A61" t="s">
+        <v>189</v>
+      </c>
+      <c r="B61" t="s">
+        <v>234</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" hidden="1">
+      <c r="A62" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" t="s">
+        <v>233</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" hidden="1">
+      <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" hidden="1">
+      <c r="A64" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" t="s">
+        <v>249</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" hidden="1">
+      <c r="A65" t="s">
+        <v>193</v>
+      </c>
+      <c r="B65" t="s">
+        <v>250</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" t="s">
+        <v>265</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>195</v>
+      </c>
+      <c r="B67" t="s">
+        <v>265</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" t="s">
+        <v>266</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>197</v>
+      </c>
+      <c r="B69" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>198</v>
+      </c>
+      <c r="B70" t="s">
+        <v>266</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>199</v>
+      </c>
+      <c r="B71" t="s">
+        <v>267</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>200</v>
+      </c>
+      <c r="B72" t="s">
+        <v>267</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" t="s">
+        <v>266</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74" t="s">
+        <v>266</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>203</v>
+      </c>
+      <c r="B75" t="s">
+        <v>266</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" t="s">
+        <v>234</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>205</v>
+      </c>
+      <c r="B77" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>206</v>
+      </c>
+      <c r="B78" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>207</v>
+      </c>
+      <c r="B79" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>208</v>
+      </c>
+      <c r="B80" t="s">
+        <v>267</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>209</v>
+      </c>
+      <c r="B81" t="s">
+        <v>266</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>210</v>
+      </c>
+      <c r="B82" t="s">
+        <v>266</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>211</v>
+      </c>
+      <c r="B83" t="s">
+        <v>234</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>212</v>
+      </c>
+      <c r="B84" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>213</v>
+      </c>
+      <c r="B85" t="s">
+        <v>234</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" t="s">
+        <v>234</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" t="s">
+        <v>266</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>216</v>
+      </c>
+      <c r="B88" t="s">
+        <v>267</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>217</v>
+      </c>
+      <c r="B89" t="s">
+        <v>266</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>281</v>
+      </c>
+      <c r="B90" t="s">
+        <v>234</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>285</v>
+      </c>
+      <c r="B91" t="s">
+        <v>234</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="Global Solar Atlas " xr:uid="{2C5A5A9E-4C70-8149-A8B9-996A26BBC283}"/>
+    <hyperlink ref="C5" r:id="rId2" display="Global Solar Atlas " xr:uid="{C1CA40AF-2DC5-7349-86F8-C77BBF78C8C3}"/>
+    <hyperlink ref="C6" location="'Slope Gradients'!A1" display="'Slope Gradients'!A1" xr:uid="{EE823616-BE43-8B4D-AFC7-C6471A85E062}"/>
+    <hyperlink ref="C15" location="'Land Cover Classes'!A1" display="'Land Cover Classes'!A1" xr:uid="{D3CD1EF9-5419-6443-ACAF-9C8278A47DA9}"/>
+    <hyperlink ref="C38" r:id="rId3" xr:uid="{BCE01F8E-9319-DB48-A386-5AEB9B177BE4}"/>
+    <hyperlink ref="C39" r:id="rId4" xr:uid="{DD8A98F4-A768-2040-8E30-CE33AFB099CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FD056C-5D0E-DF4C-88F1-1298AE9698DA}">
+  <dimension ref="A1:C162"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
@@ -962,7 +2296,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>288</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>43</v>
@@ -1405,7 +2739,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C41">
         <v>3.338348758</v>
@@ -1427,7 +2761,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C43">
         <v>3.720043639</v>
@@ -1449,7 +2783,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C45">
         <v>0.111606976</v>
@@ -1460,7 +2794,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C46">
         <v>10</v>
@@ -1471,7 +2805,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47">
         <v>9.3581930440000001</v>
@@ -1490,7 +2824,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C49">
         <v>10</v>
@@ -1501,7 +2835,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C50">
         <v>9.3581930440000001</v>
@@ -1520,7 +2854,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52">
         <v>10</v>
@@ -1531,7 +2865,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C53">
         <v>9.3581930440000001</v>
@@ -1550,7 +2884,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55">
         <v>10</v>
@@ -1561,7 +2895,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C56">
         <v>12.03970043</v>
@@ -1580,7 +2914,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -1591,7 +2925,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C59">
         <v>20</v>
@@ -1610,7 +2944,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C61">
         <v>10</v>
@@ -1621,7 +2955,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C62">
         <v>20</v>
@@ -1640,7 +2974,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64">
         <v>10</v>
@@ -1651,7 +2985,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C65">
         <v>20</v>
@@ -1670,7 +3004,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C67">
         <v>10</v>
@@ -1681,7 +3015,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C68">
         <v>20</v>
@@ -1700,7 +3034,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C70">
         <v>10</v>
@@ -1711,7 +3045,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C71">
         <v>20</v>
@@ -1730,7 +3064,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C73">
         <v>10</v>
@@ -1741,7 +3075,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C74">
         <v>20</v>
@@ -1760,7 +3094,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C76">
         <v>10</v>
@@ -1771,7 +3105,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C77">
         <v>20</v>
@@ -1790,7 +3124,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C79">
         <v>10</v>
@@ -1801,7 +3135,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80">
         <v>20</v>
@@ -1820,7 +3154,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82">
         <v>10</v>
@@ -1831,7 +3165,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C83">
         <v>20</v>
@@ -1850,7 +3184,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C85">
         <v>10</v>
@@ -1861,7 +3195,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C86">
         <v>20</v>
@@ -1880,7 +3214,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C88">
         <v>10</v>
@@ -1891,7 +3225,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C89">
         <v>20</v>
@@ -1910,7 +3244,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C91">
         <v>10</v>
@@ -1921,7 +3255,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C92">
         <v>20</v>
@@ -1940,7 +3274,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C94">
         <v>10</v>
@@ -1951,7 +3285,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C95">
         <v>20</v>
@@ -1970,7 +3304,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C97">
         <v>10</v>
@@ -1981,7 +3315,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C98">
         <v>20</v>
@@ -2000,7 +3334,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C100">
         <v>10</v>
@@ -2011,7 +3345,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C101">
         <v>20</v>
@@ -2030,7 +3364,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C103">
         <v>10</v>
@@ -2041,7 +3375,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C104">
         <v>20</v>
@@ -2060,7 +3394,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C106">
         <v>10</v>
@@ -2071,7 +3405,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C107">
         <v>20</v>
@@ -2090,7 +3424,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C109">
         <v>10</v>
@@ -2101,7 +3435,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C110">
         <v>20</v>
@@ -2120,7 +3454,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C112">
         <v>10</v>
@@ -2131,7 +3465,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C113">
         <v>20</v>
@@ -2150,7 +3484,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C115">
         <v>10</v>
@@ -2161,7 +3495,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C116">
         <v>20</v>
@@ -2180,7 +3514,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C118">
         <v>10</v>
@@ -2191,7 +3525,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C119">
         <v>20</v>
@@ -2210,7 +3544,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C121">
         <v>10</v>
@@ -2221,7 +3555,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C122">
         <v>20</v>
@@ -2240,7 +3574,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C124">
         <v>10</v>
@@ -2251,7 +3585,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C125">
         <v>20</v>
@@ -2270,7 +3604,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C127">
         <v>10</v>
@@ -2281,7 +3615,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C128">
         <v>20</v>
@@ -2300,7 +3634,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C130">
         <v>10</v>
@@ -2311,7 +3645,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C131">
         <v>20</v>
@@ -2330,7 +3664,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C133">
         <v>10</v>
@@ -2341,7 +3675,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C134">
         <v>20</v>
@@ -2360,7 +3694,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C136">
         <v>10</v>
@@ -2371,7 +3705,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C137">
         <v>20</v>
@@ -2390,7 +3724,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C139">
         <v>10</v>
@@ -2401,7 +3735,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C140">
         <v>20</v>
@@ -2420,7 +3754,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C142">
         <v>10</v>
@@ -2431,7 +3765,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C143">
         <v>20</v>
@@ -2450,7 +3784,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C145">
         <v>10</v>
@@ -2461,7 +3795,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C146">
         <v>20</v>
@@ -2480,7 +3814,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C148">
         <v>10</v>
@@ -2491,7 +3825,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C149">
         <v>20</v>
@@ -2510,7 +3844,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C151">
         <v>10</v>
@@ -2521,7 +3855,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C152">
         <v>20</v>
@@ -2540,7 +3874,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C154">
         <v>10</v>
@@ -2551,7 +3885,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C155">
         <v>20</v>
@@ -2570,7 +3904,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C157">
         <v>10</v>
@@ -2581,7 +3915,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C158">
         <v>20</v>
@@ -2600,7 +3934,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C160">
         <v>10</v>
@@ -2611,7 +3945,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C161">
         <v>20</v>
@@ -2630,7 +3964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0CFE7C-E3C5-5546-B60A-41A70AAAB55D}">
   <dimension ref="A1:G50"/>
   <sheetViews>
@@ -2644,7 +3978,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="D1" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E1" s="13"/>
     </row>
@@ -2657,10 +3991,10 @@
         <v>50</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>158</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -3263,19 +4597,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898EBC2B-50BB-1441-848C-6747EAF21234}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="D1" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E1" s="13"/>
     </row>
@@ -3287,10 +4621,10 @@
         <v>47</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>161</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>